<commit_message>
Make MultiThread Issue : printf is errer in crt
</commit_message>
<xml_diff>
--- a/MultipleFile.xlsx
+++ b/MultipleFile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Total File Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,6 +50,10 @@
   </si>
   <si>
     <t>Test Text : Big Dummy's Guide to the Internet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time(Just Search, 4 Thread) in Release</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -375,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -386,9 +390,10 @@
     <col min="1" max="1" width="15.09765625" customWidth="1"/>
     <col min="2" max="2" width="32.19921875" customWidth="1"/>
     <col min="3" max="3" width="39.59765625" customWidth="1"/>
+    <col min="4" max="4" width="35.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -396,7 +401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B2">
         <v>467333476</v>
       </c>
@@ -404,7 +409,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -412,7 +417,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -422,8 +427,11 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -435,8 +443,12 @@
         <f>AVERAGE(C8:C107)</f>
         <v>1.3934000000000006</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D7">
+        <f>AVERAGE(D8:D107)</f>
+        <v>0.28058000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -446,8 +458,11 @@
       <c r="C8">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D8">
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>2</v>
       </c>
@@ -457,8 +472,11 @@
       <c r="C9">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D9">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>3</v>
       </c>
@@ -468,8 +486,11 @@
       <c r="C10">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D10">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>4</v>
       </c>
@@ -479,8 +500,11 @@
       <c r="C11">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D11">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>5</v>
       </c>
@@ -490,8 +514,11 @@
       <c r="C12">
         <v>1.19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D12">
+        <v>0.28100000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>6</v>
       </c>
@@ -501,8 +528,11 @@
       <c r="C13">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D13">
+        <v>0.28100000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>7</v>
       </c>
@@ -512,8 +542,11 @@
       <c r="C14">
         <v>1.19</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D14">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>8</v>
       </c>
@@ -523,8 +556,11 @@
       <c r="C15">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D15">
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>9</v>
       </c>
@@ -534,8 +570,11 @@
       <c r="C16">
         <v>1.19</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D16">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>10</v>
       </c>
@@ -545,8 +584,11 @@
       <c r="C17">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D17">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>11</v>
       </c>
@@ -556,8 +598,11 @@
       <c r="C18">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D18">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>12</v>
       </c>
@@ -567,8 +612,11 @@
       <c r="C19">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D19">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>13</v>
       </c>
@@ -578,8 +626,11 @@
       <c r="C20">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D20">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>14</v>
       </c>
@@ -589,8 +640,11 @@
       <c r="C21">
         <v>1.44</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D21">
+        <v>0.26800000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>15</v>
       </c>
@@ -600,8 +654,11 @@
       <c r="C22">
         <v>1.46</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D22">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>16</v>
       </c>
@@ -611,8 +668,11 @@
       <c r="C23">
         <v>1.53</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D23">
+        <v>0.248</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>17</v>
       </c>
@@ -622,8 +682,11 @@
       <c r="C24">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D24">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>18</v>
       </c>
@@ -633,8 +696,11 @@
       <c r="C25">
         <v>1.41</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D25">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>19</v>
       </c>
@@ -644,8 +710,11 @@
       <c r="C26">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D26">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>20</v>
       </c>
@@ -655,8 +724,11 @@
       <c r="C27">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D27">
+        <v>0.25800000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>21</v>
       </c>
@@ -666,8 +738,11 @@
       <c r="C28">
         <v>1.32</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D28">
+        <v>0.26200000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>22</v>
       </c>
@@ -677,8 +752,11 @@
       <c r="C29">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D29">
+        <v>0.251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>23</v>
       </c>
@@ -688,8 +766,11 @@
       <c r="C30">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D30">
+        <v>0.26200000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>24</v>
       </c>
@@ -699,8 +780,11 @@
       <c r="C31">
         <v>1.29</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D31">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>25</v>
       </c>
@@ -710,8 +794,11 @@
       <c r="C32">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D32">
+        <v>0.25900000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>26</v>
       </c>
@@ -721,8 +808,11 @@
       <c r="C33">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D33">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>27</v>
       </c>
@@ -732,8 +822,11 @@
       <c r="C34">
         <v>1.39</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D34">
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>28</v>
       </c>
@@ -743,8 +836,11 @@
       <c r="C35">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D35">
+        <v>0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>29</v>
       </c>
@@ -754,8 +850,11 @@
       <c r="C36">
         <v>1.91</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D36">
+        <v>0.26800000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>30</v>
       </c>
@@ -765,8 +864,11 @@
       <c r="C37">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D37">
+        <v>0.26200000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>31</v>
       </c>
@@ -776,8 +878,11 @@
       <c r="C38">
         <v>1.37</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D38">
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>32</v>
       </c>
@@ -787,8 +892,11 @@
       <c r="C39">
         <v>1.54</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D39">
+        <v>0.254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>33</v>
       </c>
@@ -798,8 +906,11 @@
       <c r="C40">
         <v>1.61</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D40">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>34</v>
       </c>
@@ -809,8 +920,11 @@
       <c r="C41">
         <v>1.67</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D41">
+        <v>0.26100000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>35</v>
       </c>
@@ -820,8 +934,11 @@
       <c r="C42">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D42">
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>36</v>
       </c>
@@ -831,8 +948,11 @@
       <c r="C43">
         <v>1.43</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D43">
+        <v>0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>37</v>
       </c>
@@ -842,8 +962,11 @@
       <c r="C44">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D44">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>38</v>
       </c>
@@ -853,8 +976,11 @@
       <c r="C45">
         <v>1.57</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D45">
+        <v>0.27900000000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>39</v>
       </c>
@@ -864,8 +990,11 @@
       <c r="C46">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D46">
+        <v>0.26300000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>40</v>
       </c>
@@ -875,8 +1004,11 @@
       <c r="C47">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D47">
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>41</v>
       </c>
@@ -886,8 +1018,11 @@
       <c r="C48">
         <v>1.49</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D48">
+        <v>0.28100000000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>42</v>
       </c>
@@ -897,8 +1032,11 @@
       <c r="C49">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D49">
+        <v>0.30099999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>43</v>
       </c>
@@ -908,8 +1046,11 @@
       <c r="C50">
         <v>1.39</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D50">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>44</v>
       </c>
@@ -919,8 +1060,11 @@
       <c r="C51">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D51">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>45</v>
       </c>
@@ -930,8 +1074,11 @@
       <c r="C52">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D52">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>46</v>
       </c>
@@ -941,8 +1088,11 @@
       <c r="C53">
         <v>1.93</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D53">
+        <v>0.28100000000000003</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>47</v>
       </c>
@@ -952,8 +1102,11 @@
       <c r="C54">
         <v>1.56</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D54">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>48</v>
       </c>
@@ -963,8 +1116,11 @@
       <c r="C55">
         <v>1.43</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D55">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>49</v>
       </c>
@@ -974,8 +1130,11 @@
       <c r="C56">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D56">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>50</v>
       </c>
@@ -985,8 +1144,11 @@
       <c r="C57">
         <v>1.29</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D57">
+        <v>0.29599999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>51</v>
       </c>
@@ -996,8 +1158,11 @@
       <c r="C58">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D58">
+        <v>0.27700000000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>52</v>
       </c>
@@ -1007,8 +1172,11 @@
       <c r="C59">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D59">
+        <v>0.27100000000000002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>53</v>
       </c>
@@ -1018,8 +1186,11 @@
       <c r="C60">
         <v>1.53</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D60">
+        <v>0.28599999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>54</v>
       </c>
@@ -1029,8 +1200,11 @@
       <c r="C61">
         <v>1.28</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D61">
+        <v>0.28699999999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>55</v>
       </c>
@@ -1040,8 +1214,11 @@
       <c r="C62">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D62">
+        <v>0.28199999999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>56</v>
       </c>
@@ -1051,8 +1228,11 @@
       <c r="C63">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D63">
+        <v>0.27300000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>57</v>
       </c>
@@ -1062,8 +1242,11 @@
       <c r="C64">
         <v>1.49</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D64">
+        <v>0.28299999999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>58</v>
       </c>
@@ -1073,8 +1256,11 @@
       <c r="C65">
         <v>1.73</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D65">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>59</v>
       </c>
@@ -1084,8 +1270,11 @@
       <c r="C66">
         <v>1.64</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D66">
+        <v>0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>60</v>
       </c>
@@ -1095,8 +1284,11 @@
       <c r="C67">
         <v>1.63</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D67">
+        <v>0.29599999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>61</v>
       </c>
@@ -1106,8 +1298,11 @@
       <c r="C68">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D68">
+        <v>0.27300000000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>62</v>
       </c>
@@ -1117,8 +1312,11 @@
       <c r="C69">
         <v>1.31</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D69">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>63</v>
       </c>
@@ -1128,8 +1326,11 @@
       <c r="C70">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D70">
+        <v>0.29399999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>64</v>
       </c>
@@ -1139,8 +1340,11 @@
       <c r="C71">
         <v>1.39</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D71">
+        <v>0.29099999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>65</v>
       </c>
@@ -1150,8 +1354,11 @@
       <c r="C72">
         <v>1.63</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D72">
+        <v>0.28599999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>66</v>
       </c>
@@ -1161,8 +1368,11 @@
       <c r="C73">
         <v>1.43</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D73">
+        <v>0.317</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>67</v>
       </c>
@@ -1172,8 +1382,11 @@
       <c r="C74">
         <v>1.26</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D74">
+        <v>0.28399999999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>68</v>
       </c>
@@ -1183,8 +1396,11 @@
       <c r="C75">
         <v>1.26</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D75">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>69</v>
       </c>
@@ -1194,8 +1410,11 @@
       <c r="C76">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D76">
+        <v>0.28599999999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>70</v>
       </c>
@@ -1205,8 +1424,11 @@
       <c r="C77">
         <v>1.44</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D77">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>71</v>
       </c>
@@ -1216,8 +1438,11 @@
       <c r="C78">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D78">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>72</v>
       </c>
@@ -1227,8 +1452,11 @@
       <c r="C79">
         <v>1.33</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D79">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>73</v>
       </c>
@@ -1238,8 +1466,11 @@
       <c r="C80">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D80">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>74</v>
       </c>
@@ -1249,8 +1480,11 @@
       <c r="C81">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D81">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>75</v>
       </c>
@@ -1260,8 +1494,11 @@
       <c r="C82">
         <v>1.29</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D82">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>76</v>
       </c>
@@ -1271,8 +1508,11 @@
       <c r="C83">
         <v>1.37</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D83">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>77</v>
       </c>
@@ -1282,8 +1522,11 @@
       <c r="C84">
         <v>1.56</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D84">
+        <v>0.29399999999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>78</v>
       </c>
@@ -1293,8 +1536,11 @@
       <c r="C85">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D85">
+        <v>0.29899999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>79</v>
       </c>
@@ -1304,8 +1550,11 @@
       <c r="C86">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D86">
+        <v>0.28199999999999997</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>80</v>
       </c>
@@ -1315,8 +1564,11 @@
       <c r="C87">
         <v>1.44</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D87">
+        <v>0.28199999999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>81</v>
       </c>
@@ -1326,8 +1578,11 @@
       <c r="C88">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D88">
+        <v>0.28399999999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A89">
         <v>82</v>
       </c>
@@ -1337,8 +1592,11 @@
       <c r="C89">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D89">
+        <v>0.29799999999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>83</v>
       </c>
@@ -1348,8 +1606,11 @@
       <c r="C90">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D90">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>84</v>
       </c>
@@ -1359,8 +1620,11 @@
       <c r="C91">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D91">
+        <v>0.27300000000000002</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A92">
         <v>85</v>
       </c>
@@ -1370,8 +1634,11 @@
       <c r="C92">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D92">
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>86</v>
       </c>
@@ -1381,8 +1648,11 @@
       <c r="C93">
         <v>1.43</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D93">
+        <v>0.28599999999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A94">
         <v>87</v>
       </c>
@@ -1392,8 +1662,11 @@
       <c r="C94">
         <v>1.29</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D94">
+        <v>0.28599999999999998</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>88</v>
       </c>
@@ -1403,8 +1676,11 @@
       <c r="C95">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D95">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A96">
         <v>89</v>
       </c>
@@ -1414,8 +1690,11 @@
       <c r="C96">
         <v>1.29</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D96">
+        <v>0.28699999999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>90</v>
       </c>
@@ -1425,8 +1704,11 @@
       <c r="C97">
         <v>1.29</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D97">
+        <v>0.28299999999999997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>91</v>
       </c>
@@ -1436,8 +1718,11 @@
       <c r="C98">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D98">
+        <v>0.28599999999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A99">
         <v>92</v>
       </c>
@@ -1447,8 +1732,11 @@
       <c r="C99">
         <v>1.47</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D99">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>93</v>
       </c>
@@ -1458,8 +1746,11 @@
       <c r="C100">
         <v>1.36</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D100">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A101">
         <v>94</v>
       </c>
@@ -1469,8 +1760,11 @@
       <c r="C101">
         <v>1.26</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D101">
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>95</v>
       </c>
@@ -1480,8 +1774,11 @@
       <c r="C102">
         <v>1.28</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D102">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A103">
         <v>96</v>
       </c>
@@ -1491,8 +1788,11 @@
       <c r="C103">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D103">
+        <v>0.29799999999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>97</v>
       </c>
@@ -1502,8 +1802,11 @@
       <c r="C104">
         <v>1.32</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D104">
+        <v>0.29099999999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>98</v>
       </c>
@@ -1513,8 +1816,11 @@
       <c r="C105">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D105">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A106">
         <v>99</v>
       </c>
@@ -1524,8 +1830,11 @@
       <c r="C106">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="D106">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>100</v>
       </c>
@@ -1534,6 +1843,9 @@
       </c>
       <c r="C107">
         <v>1.34</v>
+      </c>
+      <c r="D107">
+        <v>0.28199999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>